<commit_message>
SF POC Files and Changes
SF POC Files and Changes
</commit_message>
<xml_diff>
--- a/src/resources/data/testData.xlsx
+++ b/src/resources/data/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\node\playwright-sample-project\src\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\604557499\VS Code\playwright-sample-project\src\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5AD55D1-A003-4843-B7B5-A637064473C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849EFBE6-CD05-4EF6-8AE9-06DEBB48EA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="734" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" tabRatio="881" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="RESTUserTest" sheetId="8" r:id="rId5"/>
     <sheet name="SOAPAccountServiceTest" sheetId="11" r:id="rId6"/>
     <sheet name="DatabaseTest" sheetId="10" r:id="rId7"/>
+    <sheet name="SFLoginTest" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="167">
   <si>
     <t>TestID</t>
   </si>
@@ -510,6 +511,30 @@
   </si>
   <si>
     <t>JamesB</t>
+  </si>
+  <si>
+    <t>TC01_SF_ValidLogin</t>
+  </si>
+  <si>
+    <t>dineshk.krishnamurthy@nbcuni.com.uat</t>
+  </si>
+  <si>
+    <t>*Gtrc$1234</t>
+  </si>
+  <si>
+    <t>Login to SF with valid credentials</t>
+  </si>
+  <si>
+    <t>SFLoginTest</t>
+  </si>
+  <si>
+    <t>TC04_ValidLogin</t>
+  </si>
+  <si>
+    <t>TC05_InValidLogin</t>
+  </si>
+  <si>
+    <t>TC06_LoginCreateAccount</t>
   </si>
 </sst>
 </file>
@@ -852,20 +877,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -876,51 +901,51 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -931,34 +956,45 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>156</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Run Option" error="Run column should be either 'YES' or 'NO'" sqref="B2" xr:uid="{FA756C75-86BA-4E10-996B-80241A6F0698}">
-      <formula1>"YES,NO"</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C66" xr:uid="{B00AFFEC-E6C4-4B79-86BA-26737B23EAA8}">
       <formula1>"serial,parallel"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Run Option" error="Run column should be either 'Y' OR 'N'" sqref="B3:B66" xr:uid="{7397AF50-1C00-40B0-94A9-956DA614AC6A}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Run Option" error="Run column should be either 'Y' OR 'N'" sqref="B2:B66" xr:uid="{7397AF50-1C00-40B0-94A9-956DA614AC6A}">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -975,27 +1011,27 @@
       <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="1"/>
+    <col min="15" max="15" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1078,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1089,7 +1125,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -1154,19 +1190,19 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.5546875" customWidth="1"/>
-    <col min="8" max="8" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.5703125" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1192,7 +1228,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -1218,7 +1254,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1256,22 +1292,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A954124-2682-439B-BF75-C124F90C5D43}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1291,7 +1327,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1308,7 +1344,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1328,7 +1364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1342,6 +1378,60 @@
         <v>158</v>
       </c>
       <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5">
+        <v>1243</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6">
+        <v>1244</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7">
+        <v>1245</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1359,19 +1449,19 @@
       <selection activeCell="B1" sqref="B1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1487,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1421,7 +1511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1445,7 +1535,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1471,7 +1561,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1497,7 +1587,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1523,7 +1613,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1560,19 +1650,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1598,7 +1688,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1624,7 +1714,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -1650,7 +1740,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -1676,7 +1766,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -1720,16 +1810,16 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="102.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="102.42578125" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1833,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>113</v>
       </c>
@@ -1757,7 +1847,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>117</v>
       </c>
@@ -1771,7 +1861,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>120</v>
       </c>
@@ -1785,7 +1875,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>125</v>
       </c>
@@ -1799,7 +1889,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>122</v>
       </c>
@@ -1813,7 +1903,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>129</v>
       </c>
@@ -1827,7 +1917,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>130</v>
       </c>
@@ -1845,4 +1935,67 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{156D7A28-988E-4AC3-8717-1C78F743C3E8}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2">
+        <v>1243</v>
+      </c>
+      <c r="C2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5919B0DC-35DF-46EE-8787-F7432D166336}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>